<commit_message>
Readme.md:Minor Changes to Schedule
</commit_message>
<xml_diff>
--- a/Resources/Techlauncher Semester 1.xlsx
+++ b/Resources/Techlauncher Semester 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalai\Study\COMP3500\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalai\Study\COMP3500\Master\Eye-Gaze-Technology\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DA5408E-8828-4EF4-9CDD-977466E249C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE40D638-0BE4-41AA-8E41-0FDAA9BA63C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{98EE30B1-F55F-436B-9D23-DB0A4EDC5E0B}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>H.W 2</t>
   </si>
   <si>
-    <t>Stage 3: Adding Sound &amp; Face Selection Sensitivity Settings</t>
-  </si>
-  <si>
     <t>Stage 5: Testing &amp; stabilisation</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
   </si>
   <si>
     <t>Stage &amp; Deliverable</t>
-  </si>
-  <si>
-    <t>Stage 1: Yes or No app which uses Face Selection Feature</t>
   </si>
   <si>
     <t>Note/Other Deliverable</t>
@@ -221,6 +215,12 @@
       <t xml:space="preserve">
 Integrated Testing using espresso</t>
     </r>
+  </si>
+  <si>
+    <t>Stage 1: Yes or No app which uses Face Tracking as Input</t>
+  </si>
+  <si>
+    <t>Stage 3: Adding Sound &amp; Input Sensitivity Settings</t>
   </si>
 </sst>
 </file>
@@ -361,80 +361,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,7 +756,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,136 +767,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7">
+        <v>3</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7">
+        <v>4</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="12">
+        <v>5</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="16">
-        <v>3</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="12">
+        <v>6</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="16">
-        <v>4</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="21">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="26" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="21">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="18">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="17">
-        <v>10</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Readme.md: Updated Deliverable,Added Detailed Schedule
</commit_message>
<xml_diff>
--- a/Resources/Techlauncher Semester 1.xlsx
+++ b/Resources/Techlauncher Semester 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalai\Study\COMP3500\Master\Eye-Gaze-Technology\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C952C7-C905-4E44-A525-8470949D013E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EA53FE36-26E9-47CD-A141-08A4B8542A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2630" windowWidth="14400" windowHeight="7360" xr2:uid="{98EE30B1-F55F-436B-9D23-DB0A4EDC5E0B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{98EE30B1-F55F-436B-9D23-DB0A4EDC5E0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -39,21 +39,12 @@
     <t>Project Audit 1</t>
   </si>
   <si>
-    <t>Stage 2: Basic Skeleton of App</t>
-  </si>
-  <si>
     <t>Project Audit 2</t>
   </si>
   <si>
-    <t>Stage 4: Customisable content feature</t>
-  </si>
-  <si>
     <t>Project Audit 3</t>
   </si>
   <si>
-    <t>Stage 6: Finalisation</t>
-  </si>
-  <si>
     <t>Stages</t>
   </si>
   <si>
@@ -69,13 +60,22 @@
     <t>B.W 2</t>
   </si>
   <si>
-    <t>Stage 3:Minimum Viable Product</t>
-  </si>
-  <si>
     <t>Stage 5: Integrated Testing &amp; Stabilisation</t>
   </si>
   <si>
-    <t>Stage 1:  Prototype</t>
+    <t>Stage 1:  Research &amp; Exploratory Measure</t>
+  </si>
+  <si>
+    <t>Stage 2: Prototype</t>
+  </si>
+  <si>
+    <t>4 &amp; 5</t>
+  </si>
+  <si>
+    <t>Stage 3:Basic Skeleton of the App</t>
+  </si>
+  <si>
+    <t>Stage 4: Minimum Viable Product</t>
   </si>
 </sst>
 </file>
@@ -98,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,12 +125,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -142,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -191,11 +185,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -205,24 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,9 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -245,16 +270,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B30066-FEF7-4D31-8362-9B59325FD041}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,121 +623,123 @@
     <col min="3" max="3" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>7</v>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14">
         <v>3</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6">
-        <v>4</v>
-      </c>
-      <c r="B3" s="22"/>
+    <row r="3" spans="1:6" ht="12.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="10">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="15">
         <v>5</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>1</v>
+      <c r="B4" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="10">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15">
         <v>6</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="13" t="s">
-        <v>2</v>
+      <c r="B5" s="9"/>
+      <c r="C5" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>11</v>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="18"/>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="14">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>3</v>
+      <c r="B8" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="14">
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="8">
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="B10" s="20"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7">
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>4</v>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>2</v>
       </c>
       <c r="D11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
     <mergeCell ref="B2:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>